<commit_message>
python dataTransfer and toMySQL success!
</commit_message>
<xml_diff>
--- a/code/jqForGraduation/python/testData/TesterRate.xlsx
+++ b/code/jqForGraduation/python/testData/TesterRate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
   <si>
     <t>色泽</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>耐泡性</t>
-  </si>
-  <si>
-    <t>没有</t>
   </si>
   <si>
     <t>TesterId</t>
@@ -481,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW8"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AL15" sqref="AL15"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AT3" sqref="AT3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -917,8 +914,8 @@
       <c r="AS3" s="4">
         <v>4.2</v>
       </c>
-      <c r="AT3" s="4" t="s">
-        <v>8</v>
+      <c r="AT3" s="4">
+        <v>4.4000000000000004</v>
       </c>
       <c r="AU3" s="4">
         <v>4.4000000000000004</v>
@@ -1686,7 +1683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -1694,16 +1691,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -1714,7 +1711,7 @@
         <v>1001</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -1725,7 +1722,7 @@
         <v>1001</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -1736,7 +1733,7 @@
         <v>1001</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -1747,7 +1744,7 @@
         <v>1001</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -1758,7 +1755,7 @@
         <v>1001</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
@@ -1769,7 +1766,7 @@
         <v>1001</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
@@ -1780,7 +1777,7 @@
         <v>1001</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
@@ -1791,7 +1788,7 @@
         <v>1001</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>